<commit_message>
Added graphs to document
</commit_message>
<xml_diff>
--- a/Deliverable 2/Results.xlsx
+++ b/Deliverable 2/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\dissertation\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3281B3B2-1C10-4400-A026-33EE6DDF5501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42AEA04-F34B-4283-A0F5-831EF3F4E9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="333" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="333" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="60">
   <si>
     <t>kernels/mandelbulb.cl</t>
   </si>
@@ -216,6 +216,9 @@
   <si>
     <t>kernels/benchmarks/sierpinski_hard_shadows.cl</t>
   </si>
+  <si>
+    <t>Mean Frame Time (s)</t>
+  </si>
 </sst>
 </file>
 
@@ -319,8 +322,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>title</a:t>
+              <a:t>Mandelbulb Benchmark</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> on Various Computers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -659,7 +667,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Average Frames per Second</a:t>
+                  <a:t>Mean Frames per Second (FPS)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1391,7 +1399,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>title</a:t>
+              <a:t>Mandelbulb Benchmark using Various Resolutions</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1730,7 +1738,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Average Frames per Second</a:t>
+                  <a:t>Mean Frames per Second (FPS)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5880,16 +5888,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6330,8 +6338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668D4FD2-0EC3-4246-9368-74132FA6B2E6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7069,8 +7077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2244C4-2775-4810-AA43-487CC5A15D7E}">
   <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7168,7 +7176,7 @@
         <v>28</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>50</v>
@@ -7846,8 +7854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F5E1FA-4FA3-4867-B8E6-04C4F7C4055D}">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7933,7 +7941,7 @@
         <v>28</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Big progress on the report
</commit_message>
<xml_diff>
--- a/Deliverable 2/Results.xlsx
+++ b/Deliverable 2/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\dissertation\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42AEA04-F34B-4283-A0F5-831EF3F4E9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2194E1-9497-40F5-AA54-19540AD5D55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="333" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="333" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="2" r:id="rId1"/>
@@ -1935,7 +1935,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Scene Optimisations and Features</a:t>
+              <a:t> Scene Optimisations</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1993,12 +1993,32 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Mandelbulb!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Basic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bounding volume optimisation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Linear epsilon optimisation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fast maths optimisation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mandelbulb!$Y$2:$Y$8</c:f>
+              <c:f>Mandelbulb!$Y$2:$Y$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>43.778236962841035</c:v>
                 </c:pt>
@@ -2010,15 +2030,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>80.776749220504371</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>67.490045218330295</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>39.099766965388888</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>53.923762584458089</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2047,9 +2058,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Mandelbulb!$A$2:$A$8</c:f>
+              <c:f>Mandelbulb!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Basic</c:v>
                 </c:pt>
@@ -2061,25 +2072,16 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Fast maths optimisation</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Phong shading</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Hard shadows</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>All features</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mandelbulb!$X$2:$X$8</c:f>
+              <c:f>Mandelbulb!$X$2:$X$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>26.341186198139987</c:v>
                 </c:pt>
@@ -2091,15 +2093,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>49.069473662632632</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.723713262603546</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29.662417102765676</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31.35935776035307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2126,12 +2119,32 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Mandelbulb!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Basic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bounding volume optimisation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Linear epsilon optimisation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fast maths optimisation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mandelbulb!$Z$2:$Z$8</c:f>
+              <c:f>Mandelbulb!$Z$2:$Z$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>18.84062339854701</c:v>
                 </c:pt>
@@ -2143,15 +2156,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5.2095543226276995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33.04135786764293</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23.420849239993444</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>22.199233682453283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2814,6 +2818,571 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-55E6-482B-9FAA-335A91CBB004}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="229290624"/>
+        <c:axId val="228701984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="229290624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Optimisations/Features</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="228701984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="228701984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frames Per Second (FPS)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="229290624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Mandelbulb</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Features</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Max FPS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Mandelbulb!$A$6:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Phong shading</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hard shadows</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>All features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Mandelbulb!$Y$6:$Y$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>67.490045218330295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.099766965388888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.923762584458089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AEBA-4861-BBAB-4063B4AD157A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mean FPS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Mandelbulb!$A$6:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Phong shading</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hard shadows</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>All features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Mandelbulb!$X$6:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43.723713262603546</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.662417102765676</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.35935776035307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AEBA-4861-BBAB-4063B4AD157A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Min FPS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Mandelbulb!$A$6:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Phong shading</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hard shadows</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>All features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Mandelbulb!$Z$6:$Z$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>33.04135786764293</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.420849239993444</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.199233682453283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AEBA-4861-BBAB-4063B4AD157A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3330,6 +3899,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5382,6 +5991,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5999,15 +7111,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6034,16 +7146,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
+      <xdr:col>40</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>115659</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6065,6 +7177,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F417B0DF-6127-4924-998B-8E4A8A422382}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6338,8 +7488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668D4FD2-0EC3-4246-9368-74132FA6B2E6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7077,8 +8227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2244C4-2775-4810-AA43-487CC5A15D7E}">
   <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7854,7 +9004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F5E1FA-4FA3-4867-B8E6-04C4F7C4055D}">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated sierpinski benchmark scene
</commit_message>
<xml_diff>
--- a/Deliverable 2/Results.xlsx
+++ b/Deliverable 2/Results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\dissertation\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2194E1-9497-40F5-AA54-19540AD5D55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB2A4B4-B0E6-48B9-91ED-5BEC7B6EBF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="333" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="333" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="2" r:id="rId1"/>
     <sheet name="Raw Data" sheetId="1" r:id="rId2"/>
     <sheet name="Mandelbulb" sheetId="3" r:id="rId3"/>
-    <sheet name="Sierpinski" sheetId="4" r:id="rId4"/>
+    <sheet name="Mandelbulb Optimisations" sheetId="5" r:id="rId4"/>
+    <sheet name="Sierpinski" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="65">
   <si>
     <t>kernels/mandelbulb.cl</t>
   </si>
@@ -218,6 +219,21 @@
   </si>
   <si>
     <t>Mean Frame Time (s)</t>
+  </si>
+  <si>
+    <t>Bounding Volume</t>
+  </si>
+  <si>
+    <t>Linear Epsilon</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-cl-fast-relaxed-math </t>
   </si>
 </sst>
 </file>
@@ -8227,8 +8243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2244C4-2775-4810-AA43-487CC5A15D7E}">
   <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J77" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9001,6 +9017,608 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412B021C-7FB8-4DB3-B867-3D7A2496B207}">
+  <dimension ref="A1:AB8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <v>1920</v>
+      </c>
+      <c r="E2">
+        <v>1080</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>256</v>
+      </c>
+      <c r="I2">
+        <v>1665</v>
+      </c>
+      <c r="J2">
+        <v>38</v>
+      </c>
+      <c r="K2">
+        <v>8589410304</v>
+      </c>
+      <c r="L2">
+        <v>49152</v>
+      </c>
+      <c r="M2">
+        <v>65536</v>
+      </c>
+      <c r="N2">
+        <v>39.045099999999998</v>
+      </c>
+      <c r="O2">
+        <v>502</v>
+      </c>
+      <c r="P2">
+        <v>0.101914</v>
+      </c>
+      <c r="Q2">
+        <v>5.12617E-2</v>
+      </c>
+      <c r="S2">
+        <f>D2*E2</f>
+        <v>2073600</v>
+      </c>
+      <c r="T2" s="3">
+        <f>K2/1000000000</f>
+        <v>8.5894103039999994</v>
+      </c>
+      <c r="U2" s="3">
+        <f>L2/1000</f>
+        <v>49.152000000000001</v>
+      </c>
+      <c r="V2" s="3">
+        <f>M2/1000</f>
+        <v>65.536000000000001</v>
+      </c>
+      <c r="W2">
+        <f>N2/O2</f>
+        <v>7.7779083665338644E-2</v>
+      </c>
+      <c r="X2">
+        <f>1/W2</f>
+        <v>12.856926989558229</v>
+      </c>
+      <c r="Y2">
+        <f>1/Q2</f>
+        <v>19.50774164727272</v>
+      </c>
+      <c r="Z2">
+        <f>1/P2</f>
+        <v>9.8121945954432164</v>
+      </c>
+      <c r="AA2">
+        <f>Y2-X2</f>
+        <v>6.6508146577144913</v>
+      </c>
+      <c r="AB2">
+        <f>X2-Z2</f>
+        <v>3.0447323941150124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>1920</v>
+      </c>
+      <c r="E3">
+        <v>1080</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>256</v>
+      </c>
+      <c r="I3">
+        <v>1665</v>
+      </c>
+      <c r="J3">
+        <v>38</v>
+      </c>
+      <c r="K3">
+        <v>8589410304</v>
+      </c>
+      <c r="L3">
+        <v>49152</v>
+      </c>
+      <c r="M3">
+        <v>65536</v>
+      </c>
+      <c r="N3">
+        <v>39.079700000000003</v>
+      </c>
+      <c r="O3">
+        <v>468</v>
+      </c>
+      <c r="P3">
+        <v>0.111606</v>
+      </c>
+      <c r="Q3">
+        <v>5.3742900000000003E-2</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S8" si="0">D3*E3</f>
+        <v>2073600</v>
+      </c>
+      <c r="T3" s="3">
+        <f t="shared" ref="T3:T8" si="1">K3/1000000000</f>
+        <v>8.5894103039999994</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" ref="U3:V8" si="2">L3/1000</f>
+        <v>49.152000000000001</v>
+      </c>
+      <c r="V3" s="3">
+        <f t="shared" si="2"/>
+        <v>65.536000000000001</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W8" si="3">N3/O3</f>
+        <v>8.3503632478632489E-2</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X8" si="4">1/W3</f>
+        <v>11.975526935979548</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y8" si="5">1/Q3</f>
+        <v>18.607109032076796</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z8" si="6">1/P3</f>
+        <v>8.9600917513395348</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ref="AA3:AA8" si="7">Y3-X3</f>
+        <v>6.6315820960972474</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB8" si="8">X3-Z3</f>
+        <v>3.0154351846400136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>1920</v>
+      </c>
+      <c r="E4">
+        <v>1080</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>256</v>
+      </c>
+      <c r="I4">
+        <v>1665</v>
+      </c>
+      <c r="J4">
+        <v>38</v>
+      </c>
+      <c r="K4">
+        <v>8589410304</v>
+      </c>
+      <c r="L4">
+        <v>49152</v>
+      </c>
+      <c r="M4">
+        <v>65536</v>
+      </c>
+      <c r="N4">
+        <v>39.114400000000003</v>
+      </c>
+      <c r="O4">
+        <v>623</v>
+      </c>
+      <c r="P4">
+        <v>9.4061000000000006E-2</v>
+      </c>
+      <c r="Q4">
+        <v>3.3295999999999999E-2</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>2073600</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="1"/>
+        <v>8.5894103039999994</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="2"/>
+        <v>49.152000000000001</v>
+      </c>
+      <c r="V4" s="3">
+        <f t="shared" si="2"/>
+        <v>65.536000000000001</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="3"/>
+        <v>6.2783948635634038E-2</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="4"/>
+        <v>15.927637903176322</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="5"/>
+        <v>30.033637674195099</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="6"/>
+        <v>10.631398773136581</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" si="7"/>
+        <v>14.105999771018777</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="8"/>
+        <v>5.2962391300397407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>1920</v>
+      </c>
+      <c r="E5">
+        <v>1080</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>256</v>
+      </c>
+      <c r="I5">
+        <v>1665</v>
+      </c>
+      <c r="J5">
+        <v>38</v>
+      </c>
+      <c r="K5">
+        <v>8589410304</v>
+      </c>
+      <c r="L5">
+        <v>49152</v>
+      </c>
+      <c r="M5">
+        <v>65536</v>
+      </c>
+      <c r="N5">
+        <v>39.061799999999998</v>
+      </c>
+      <c r="O5">
+        <v>993</v>
+      </c>
+      <c r="P5">
+        <v>5.3898500000000002E-2</v>
+      </c>
+      <c r="Q5">
+        <v>2.75404E-2</v>
+      </c>
+      <c r="S5">
+        <f>D6*E6</f>
+        <v>2073600</v>
+      </c>
+      <c r="T5" s="3">
+        <f>K6/1000000000</f>
+        <v>8.5894103039999994</v>
+      </c>
+      <c r="U5" s="3">
+        <f>L6/1000</f>
+        <v>49.152000000000001</v>
+      </c>
+      <c r="V5" s="3">
+        <f>M6/1000</f>
+        <v>65.536000000000001</v>
+      </c>
+      <c r="W5">
+        <f>N6/O6</f>
+        <v>3.1870938775510206E-2</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="4"/>
+        <v>31.376546735686528</v>
+      </c>
+      <c r="Y5">
+        <f>1/Q6</f>
+        <v>53.019739248922377</v>
+      </c>
+      <c r="Z5">
+        <f>1/P6</f>
+        <v>22.338930724741928</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="7"/>
+        <v>21.643192513235849</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="8"/>
+        <v>9.0376160109445998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>1920</v>
+      </c>
+      <c r="E6">
+        <v>1080</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>256</v>
+      </c>
+      <c r="I6">
+        <v>1665</v>
+      </c>
+      <c r="J6">
+        <v>38</v>
+      </c>
+      <c r="K6">
+        <v>8589410304</v>
+      </c>
+      <c r="L6">
+        <v>49152</v>
+      </c>
+      <c r="M6">
+        <v>65536</v>
+      </c>
+      <c r="N6">
+        <v>39.041899999999998</v>
+      </c>
+      <c r="O6">
+        <v>1225</v>
+      </c>
+      <c r="P6">
+        <v>4.4764900000000003E-2</v>
+      </c>
+      <c r="Q6">
+        <v>1.88609E-2</v>
+      </c>
+      <c r="S6">
+        <f>D5*E5</f>
+        <v>2073600</v>
+      </c>
+      <c r="T6" s="3">
+        <f>K5/1000000000</f>
+        <v>8.5894103039999994</v>
+      </c>
+      <c r="U6" s="3">
+        <f>L5/1000</f>
+        <v>49.152000000000001</v>
+      </c>
+      <c r="V6" s="3">
+        <f>M5/1000</f>
+        <v>65.536000000000001</v>
+      </c>
+      <c r="W6">
+        <f>N5/O5</f>
+        <v>3.933716012084592E-2</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="4"/>
+        <v>25.421255548899438</v>
+      </c>
+      <c r="Y6">
+        <f>1/Q5</f>
+        <v>36.310293241928221</v>
+      </c>
+      <c r="Z6">
+        <f>1/P5</f>
+        <v>18.55339202389677</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="7"/>
+        <v>10.889037693028783</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="8"/>
+        <v>6.8678635250026687</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F5E1FA-4FA3-4867-B8E6-04C4F7C4055D}">
   <dimension ref="A1:AB9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Ran mandelbulb benchmark again
</commit_message>
<xml_diff>
--- a/Deliverable 2/Results.xlsx
+++ b/Deliverable 2/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\dissertation\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF41C91F-7A58-43C1-92DE-27DC02020770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC56D8C7-2EBC-4852-B46E-023791F47487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="68">
   <si>
     <t>kernels/mandelbulb.cl</t>
   </si>
@@ -168,18 +168,6 @@
     <t xml:space="preserve">-cl-fast-relaxed-math </t>
   </si>
   <si>
-    <t>kernels/benchmarks/mandelbulb_features/no_features.cl</t>
-  </si>
-  <si>
-    <t>kernels/benchmarks/mandelbulb_features/hard_shadows.cl</t>
-  </si>
-  <si>
-    <t>kernels/benchmarks/mandelbulb_features/phong.cl</t>
-  </si>
-  <si>
-    <t>kernels/benchmarks/mandelbulb_features/all_features.cl</t>
-  </si>
-  <si>
     <t>kernels/benchmarks/sierpinski_optimisations/no_optimisations.cl</t>
   </si>
   <si>
@@ -207,25 +195,55 @@
     <t>kernels/benchmarks/sierpinski_features/all_features.cl</t>
   </si>
   <si>
-    <t>kernels/benchmarks/mandelbulb_optimisations/no_optimisations.cl</t>
-  </si>
-  <si>
-    <t>kernels/benchmarks/mandelbulb_optimisations/linear_epsilon.cl</t>
-  </si>
-  <si>
-    <t>kernels/benchmarks/mandelbulb_optimisations/all_optimisations.cl</t>
-  </si>
-  <si>
     <t>Hard Shadows</t>
   </si>
   <si>
     <t>Phong</t>
   </si>
   <si>
-    <t>kernels/benchmarks/mandelbulb_optimisations/bounding_volume.cl</t>
+    <t>kernels/benchmarks/sierpinski_optimisations/bounding_volume.cl</t>
   </si>
   <si>
-    <t>kernels/benchmarks/sierpinski_optimisations/bounding_volume.cl</t>
+    <t>kernels/benchmarks/mandelbulb/optimisations_none.cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-I "kernels" -I "kernels\benchmarks" -I "kernels\benchmarks\mandelbulb" -I "kernels\benchmarks\mandelbulb_features" -I "kernels\benchmarks\mandelbulb_optimisations" -I "kernels\benchmarks\sierpinski_features" -I "kernels\benchmarks\sierpinski_optimisations" -I "kernels\include" -I "kernels/include" </t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/optimisations_intersection_epsilon.cl</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/optimisations_bounding_volume.cl</t>
+  </si>
+  <si>
+    <t>-I "kernels" -I "kernels\benchmarks" -I "kernels\benchmarks\mandelbulb" -I "kernels\benchmarks\mandelbulb_features" -I "kernels\benchmarks\mandelbulb_optimisations" -I "kernels\benchmarks\sierpinski_features" -I "kernels\benchmarks\sierpinski_optimisations" -I "kernels\include" -I "kernels/include" -cl-fast-relaxed-math</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/optimisations_all.cl</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/features_none.cl</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/features_phong.cl</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/features_glow.cl</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/features_hard_shadows.cl</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/features_soft_shadows.cl</t>
+  </si>
+  <si>
+    <t>kernels/benchmarks/mandelbulb/features_all.cl</t>
+  </si>
+  <si>
+    <t>Glow</t>
+  </si>
+  <si>
+    <t>Soft Shadows</t>
   </si>
 </sst>
 </file>
@@ -2031,19 +2049,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20.043655080765909</c:v>
+                  <c:v>20.278916213601878</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.280365907941633</c:v>
+                  <c:v>25.026528119806994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.301516713183322</c:v>
+                  <c:v>19.584188509564918</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.194601811808134</c:v>
+                  <c:v>41.699678912472379</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.548906091240688</c:v>
+                  <c:v>45.611906532081136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2100,19 +2118,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12.392531567293691</c:v>
+                  <c:v>11.754344140707776</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.138150538062874</c:v>
+                  <c:v>13.479990328852148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.303891167848487</c:v>
+                  <c:v>11.219544579433046</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.036842446973743</c:v>
+                  <c:v>23.656865648301263</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.880646932561273</c:v>
+                  <c:v>26.038635615399709</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2169,19 +2187,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.359924388204016</c:v>
+                  <c:v>7.7761102341386801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0995545940048417</c:v>
+                  <c:v>7.7054068840105101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4957420410920639</c:v>
+                  <c:v>7.550874013667082</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.800626908512768</c:v>
+                  <c:v>16.485599828549763</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.430047537567708</c:v>
+                  <c:v>16.29521719080233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2604,19 +2622,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Mandelbulb Features'!$A$2:$A$5</c:f>
+              <c:f>'Mandelbulb Features'!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Phong</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Glow</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Hard Shadows</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phong</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Soft Shadows</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>All</c:v>
                 </c:pt>
               </c:strCache>
@@ -2624,21 +2648,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Mandelbulb Features'!$Y$2:$Y$5</c:f>
+              <c:f>'Mandelbulb Features'!$Y$2:$Y$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>117.72739045466318</c:v>
+                  <c:v>111.76306230790723</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.797528171573973</c:v>
+                  <c:v>95.721259691777547</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104.23615743829218</c:v>
+                  <c:v>108.22042335829619</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.656798782574811</c:v>
+                  <c:v>47.894096573656334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45.543147578015414</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.933506655765115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2667,19 +2697,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Mandelbulb Features'!$A$2:$A$5</c:f>
+              <c:f>'Mandelbulb Features'!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Phong</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Glow</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Hard Shadows</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phong</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Soft Shadows</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>All</c:v>
                 </c:pt>
               </c:strCache>
@@ -2687,21 +2723,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Mandelbulb Features'!$X$2:$X$5</c:f>
+              <c:f>'Mandelbulb Features'!$X$2:$X$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>63.898880895283781</c:v>
+                  <c:v>64.022319585569505</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.526055086184506</c:v>
+                  <c:v>54.436074214070864</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.491557804254931</c:v>
+                  <c:v>63.875206895058831</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.961846662488171</c:v>
+                  <c:v>28.087460029383809</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.968066925128181</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.828455179153746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2730,19 +2772,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Mandelbulb Features'!$A$2:$A$5</c:f>
+              <c:f>'Mandelbulb Features'!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>None</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Phong</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Glow</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Hard Shadows</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phong</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Soft Shadows</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>All</c:v>
                 </c:pt>
               </c:strCache>
@@ -2750,21 +2798,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Mandelbulb Features'!$Z$2:$Z$5</c:f>
+              <c:f>'Mandelbulb Features'!$Z$2:$Z$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41.880431368443098</c:v>
+                  <c:v>37.646491911651211</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.045666608067723</c:v>
+                  <c:v>30.422507788161994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.855593277053167</c:v>
+                  <c:v>37.85684811453968</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.779346686229143</c:v>
+                  <c:v>17.99911084392431</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.367174649210529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.321547543851917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8645,7 +8699,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA46" sqref="AA46"/>
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9381,10 +9435,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412B021C-7FB8-4DB3-B867-3D7A2496B207}">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9505,10 +9559,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
       </c>
       <c r="D2">
         <v>1920</v>
@@ -9541,16 +9595,16 @@
         <v>65536</v>
       </c>
       <c r="N2">
-        <v>40.104799999999997</v>
+        <v>30.201599999999999</v>
       </c>
       <c r="O2">
-        <v>497</v>
+        <v>355</v>
       </c>
       <c r="P2">
-        <v>0.73533499999999996</v>
+        <v>0.12859899999999999</v>
       </c>
       <c r="Q2">
-        <v>4.9891100000000001E-2</v>
+        <v>4.9312300000000003E-2</v>
       </c>
       <c r="S2">
         <f>D2*E2</f>
@@ -9570,27 +9624,27 @@
       </c>
       <c r="W2">
         <f>N2/O2</f>
-        <v>8.0693762575452715E-2</v>
+        <v>8.5074929577464792E-2</v>
       </c>
       <c r="X2">
         <f>1/W2</f>
-        <v>12.392531567293691</v>
+        <v>11.754344140707776</v>
       </c>
       <c r="Y2">
         <f>1/Q2</f>
-        <v>20.043655080765909</v>
+        <v>20.278916213601878</v>
       </c>
       <c r="Z2">
         <f>1/P2</f>
-        <v>1.359924388204016</v>
+        <v>7.7761102341386801</v>
       </c>
       <c r="AA2">
         <f>Y2-X2</f>
-        <v>7.6511235134722178</v>
+        <v>8.5245720728941023</v>
       </c>
       <c r="AB2">
         <f>X2-Z2</f>
-        <v>11.032607179089675</v>
+        <v>3.9782339065690957</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -9601,7 +9655,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>1920</v>
@@ -9634,60 +9688,60 @@
         <v>65536</v>
       </c>
       <c r="N3">
-        <v>40.153300000000002</v>
+        <v>30.192900000000002</v>
       </c>
       <c r="O3">
-        <v>648</v>
+        <v>407</v>
       </c>
       <c r="P3">
-        <v>0.322627</v>
+        <v>0.12977900000000001</v>
       </c>
       <c r="Q3">
-        <v>3.3024699999999997E-2</v>
+        <v>3.9957600000000003E-2</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S4" si="0">D3*E3</f>
+        <f t="shared" ref="S3:S6" si="0">D3*E3</f>
         <v>2073600</v>
       </c>
       <c r="T3" s="3">
-        <f t="shared" ref="T3:T4" si="1">K3/1000000000</f>
+        <f t="shared" ref="T3:T6" si="1">K3/1000000000</f>
         <v>8.5894103039999994</v>
       </c>
       <c r="U3" s="3">
-        <f t="shared" ref="U3:V4" si="2">L3/1000</f>
+        <f t="shared" ref="U3:U6" si="2">L3/1000</f>
         <v>49.152000000000001</v>
       </c>
       <c r="V3" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="V3:V6" si="3">M3/1000</f>
         <v>65.536000000000001</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W4" si="3">N3/O3</f>
-        <v>6.1964969135802468E-2</v>
+        <f t="shared" ref="W3:W6" si="4">N3/O3</f>
+        <v>7.4184029484029482E-2</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X6" si="4">1/W3</f>
-        <v>16.138150538062874</v>
+        <f t="shared" ref="X3:X6" si="5">1/W3</f>
+        <v>13.479990328852148</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y4" si="5">1/Q3</f>
-        <v>30.280365907941633</v>
+        <f t="shared" ref="Y3:Y6" si="6">1/Q3</f>
+        <v>25.026528119806994</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z4" si="6">1/P3</f>
-        <v>3.0995545940048417</v>
+        <f t="shared" ref="Z3:Z6" si="7">1/P3</f>
+        <v>7.7054068840105101</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA6" si="7">Y3-X3</f>
-        <v>14.142215369878759</v>
+        <f t="shared" ref="AA3:AA6" si="8">Y3-X3</f>
+        <v>11.546537790954845</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB6" si="8">X3-Z3</f>
-        <v>13.038595944058033</v>
+        <f t="shared" ref="AB3:AB6" si="9">X3-Z3</f>
+        <v>5.774583444841638</v>
       </c>
       <c r="AD3">
         <f>(X3-$X$2)/ABS($X$2)*100</f>
-        <v>30.224808792536002</v>
+        <v>14.680922793200304</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -9695,10 +9749,10 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>1920</v>
@@ -9731,16 +9785,16 @@
         <v>65536</v>
       </c>
       <c r="N4">
-        <v>40.149900000000002</v>
+        <v>30.126000000000001</v>
       </c>
       <c r="O4">
-        <v>494</v>
+        <v>338</v>
       </c>
       <c r="P4">
-        <v>0.153947</v>
+        <v>0.132435</v>
       </c>
       <c r="Q4">
-        <v>5.1809399999999999E-2</v>
+        <v>5.1061599999999999E-2</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
@@ -9755,36 +9809,36 @@
         <v>49.152000000000001</v>
       </c>
       <c r="V4" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65.536000000000001</v>
       </c>
       <c r="W4">
-        <f t="shared" si="3"/>
-        <v>8.1275101214574902E-2</v>
+        <f t="shared" si="4"/>
+        <v>8.9130177514792908E-2</v>
       </c>
       <c r="X4">
-        <f t="shared" si="4"/>
-        <v>12.303891167848487</v>
+        <f t="shared" si="5"/>
+        <v>11.219544579433046</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="5"/>
-        <v>19.301516713183322</v>
+        <f t="shared" si="6"/>
+        <v>19.584188509564918</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="6"/>
-        <v>6.4957420410920639</v>
+        <f t="shared" si="7"/>
+        <v>7.550874013667082</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="7"/>
-        <v>6.9976255453348344</v>
+        <f t="shared" si="8"/>
+        <v>8.3646439301318711</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="8"/>
-        <v>5.8081491267564234</v>
+        <f t="shared" si="9"/>
+        <v>3.6686705657659644</v>
       </c>
       <c r="AD4">
         <f>(X4-$X$2)/ABS($X$2)*100</f>
-        <v>-0.71527273474245701</v>
+        <v>-4.5498035013506675</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -9792,10 +9846,10 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>1920</v>
@@ -9828,60 +9882,60 @@
         <v>65536</v>
       </c>
       <c r="N5">
-        <v>40.066000000000003</v>
+        <v>30.0547</v>
       </c>
       <c r="O5">
-        <v>1077</v>
+        <v>711</v>
       </c>
       <c r="P5">
-        <v>8.7488700000000003E-2</v>
+        <v>6.0658999999999998E-2</v>
       </c>
       <c r="Q5">
-        <v>2.7360599999999999E-2</v>
+        <v>2.3980999999999999E-2</v>
       </c>
       <c r="S5">
-        <f>D6*E6</f>
+        <f t="shared" si="0"/>
         <v>2073600</v>
       </c>
       <c r="T5" s="3">
-        <f>K6/1000000000</f>
+        <f t="shared" si="1"/>
         <v>8.5894103039999994</v>
       </c>
       <c r="U5" s="3">
-        <f>L6/1000</f>
+        <f t="shared" si="2"/>
         <v>49.152000000000001</v>
       </c>
       <c r="V5" s="3">
-        <f>M6/1000</f>
+        <f t="shared" si="3"/>
         <v>65.536000000000001</v>
       </c>
       <c r="W5">
-        <f>N6/O6</f>
-        <v>3.0269236583522298E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.2271026722925459E-2</v>
       </c>
       <c r="X5">
-        <f t="shared" si="4"/>
-        <v>33.036842446973743</v>
+        <f t="shared" si="5"/>
+        <v>23.656865648301263</v>
       </c>
       <c r="Y5">
-        <f>1/Q6</f>
-        <v>53.194601811808134</v>
+        <f t="shared" si="6"/>
+        <v>41.699678912472379</v>
       </c>
       <c r="Z5">
-        <f>1/P6</f>
-        <v>23.800626908512768</v>
+        <f t="shared" si="7"/>
+        <v>16.485599828549763</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="7"/>
-        <v>20.157759364834391</v>
+        <f t="shared" si="8"/>
+        <v>18.042813264171116</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="8"/>
-        <v>9.236215538460975</v>
+        <f t="shared" si="9"/>
+        <v>7.1712658197515005</v>
       </c>
       <c r="AD5">
-        <f t="shared" ref="AD4:AD6" si="9">(X5-$X$2)/ABS($X$2)*100</f>
-        <v>166.58671206587374</v>
+        <f t="shared" ref="AD4:AD6" si="10">(X5-$X$2)/ABS($X$2)*100</f>
+        <v>101.2606179052776</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -9889,10 +9943,10 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>1920</v>
@@ -9925,60 +9979,60 @@
         <v>65536</v>
       </c>
       <c r="N6">
-        <v>40.046199999999999</v>
+        <v>30.070699999999999</v>
       </c>
       <c r="O6">
-        <v>1323</v>
+        <v>783</v>
       </c>
       <c r="P6">
-        <v>4.2015700000000003E-2</v>
+        <v>6.1367699999999997E-2</v>
       </c>
       <c r="Q6">
-        <v>1.87989E-2</v>
+        <v>2.1924099999999998E-2</v>
       </c>
       <c r="S6">
-        <f>D5*E5</f>
+        <f t="shared" si="0"/>
         <v>2073600</v>
       </c>
       <c r="T6" s="3">
-        <f>K5/1000000000</f>
+        <f t="shared" si="1"/>
         <v>8.5894103039999994</v>
       </c>
       <c r="U6" s="3">
-        <f>L5/1000</f>
+        <f t="shared" si="2"/>
         <v>49.152000000000001</v>
       </c>
       <c r="V6" s="3">
-        <f>M5/1000</f>
+        <f t="shared" si="3"/>
         <v>65.536000000000001</v>
       </c>
       <c r="W6">
-        <f>N5/O5</f>
-        <v>3.7201485608170846E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.8404469987228608E-2</v>
       </c>
       <c r="X6">
-        <f t="shared" si="4"/>
-        <v>26.880646932561273</v>
+        <f t="shared" si="5"/>
+        <v>26.038635615399709</v>
       </c>
       <c r="Y6">
-        <f>1/Q5</f>
-        <v>36.548906091240688</v>
+        <f t="shared" si="6"/>
+        <v>45.611906532081136</v>
       </c>
       <c r="Z6">
-        <f>1/P5</f>
-        <v>11.430047537567708</v>
+        <f t="shared" si="7"/>
+        <v>16.29521719080233</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="7"/>
-        <v>9.6682591586794153</v>
+        <f t="shared" si="8"/>
+        <v>19.573270916681427</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="8"/>
-        <v>15.450599394993565</v>
+        <f t="shared" si="9"/>
+        <v>9.7434184245973796</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="9"/>
-        <v>116.91005414506705</v>
+        <f t="shared" si="10"/>
+        <v>121.52350912733971</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -9987,13 +10041,23 @@
       <c r="V7" s="3"/>
       <c r="AD7">
         <f>SUM(AD3:AD5)</f>
-        <v>196.09624812366729</v>
+        <v>111.39173719712724</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10003,16 +10067,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2244C4-2775-4810-AA43-487CC5A15D7E}">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD3:AD4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="95" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -10128,10 +10192,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>1920</v>
@@ -10164,16 +10228,16 @@
         <v>65536</v>
       </c>
       <c r="N2">
-        <v>40.031999999999996</v>
+        <v>30.0364</v>
       </c>
       <c r="O2">
-        <v>2558</v>
+        <v>1923</v>
       </c>
       <c r="P2">
-        <v>2.3877499999999999E-2</v>
+        <v>2.65629E-2</v>
       </c>
       <c r="Q2">
-        <v>8.4942000000000004E-3</v>
+        <v>8.9475000000000006E-3</v>
       </c>
       <c r="S2">
         <f>D2*E2</f>
@@ -10193,38 +10257,38 @@
       </c>
       <c r="W2">
         <f>N2/O2</f>
-        <v>1.5649726348709928E-2</v>
+        <v>1.5619552782111284E-2</v>
       </c>
       <c r="X2">
         <f>1/W2</f>
-        <v>63.898880895283781</v>
+        <v>64.022319585569505</v>
       </c>
       <c r="Y2">
         <f>1/Q2</f>
-        <v>117.72739045466318</v>
+        <v>111.76306230790723</v>
       </c>
       <c r="Z2">
         <f>1/P2</f>
-        <v>41.880431368443098</v>
+        <v>37.646491911651211</v>
       </c>
       <c r="AA2">
         <f>Y2-X2</f>
-        <v>53.828509559379398</v>
+        <v>47.740742722337728</v>
       </c>
       <c r="AB2">
         <f>X2-Z2</f>
-        <v>22.018449526840683</v>
+        <v>26.375827673918295</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
       </c>
       <c r="D3">
         <v>1920</v>
@@ -10257,71 +10321,71 @@
         <v>65536</v>
       </c>
       <c r="N3">
-        <v>40.053600000000003</v>
+        <v>30.053599999999999</v>
       </c>
       <c r="O3">
-        <v>1463</v>
+        <v>1636</v>
       </c>
       <c r="P3">
-        <v>3.69745E-2</v>
+        <v>3.2870400000000001E-2</v>
       </c>
       <c r="Q3">
-        <v>1.7606400000000001E-2</v>
+        <v>1.0447E-2</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S5" si="0">D3*E3</f>
+        <f t="shared" ref="S3:S7" si="0">D3*E3</f>
         <v>2073600</v>
       </c>
       <c r="T3" s="3">
-        <f t="shared" ref="T3:T5" si="1">K3/1000000000</f>
+        <f t="shared" ref="T3:T7" si="1">K3/1000000000</f>
         <v>8.5894103039999994</v>
       </c>
       <c r="U3" s="3">
-        <f t="shared" ref="U3:U5" si="2">L3/1000</f>
+        <f t="shared" ref="U3:U7" si="2">L3/1000</f>
         <v>49.152000000000001</v>
       </c>
       <c r="V3" s="3">
-        <f t="shared" ref="V3:V5" si="3">M3/1000</f>
+        <f t="shared" ref="V3:V7" si="3">M3/1000</f>
         <v>65.536000000000001</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W5" si="4">N3/O3</f>
-        <v>2.7377717019822286E-2</v>
+        <f t="shared" ref="W3:W7" si="4">N3/O3</f>
+        <v>1.8370171149144254E-2</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X5" si="5">1/W3</f>
-        <v>36.526055086184506</v>
+        <f t="shared" ref="X3:X7" si="5">1/W3</f>
+        <v>54.436074214070864</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y5" si="6">1/Q3</f>
-        <v>56.797528171573973</v>
+        <f t="shared" ref="Y3:Y7" si="6">1/Q3</f>
+        <v>95.721259691777547</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z5" si="7">1/P3</f>
-        <v>27.045666608067723</v>
+        <f t="shared" ref="Z3:Z7" si="7">1/P3</f>
+        <v>30.422507788161994</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA5" si="8">Y3-X3</f>
-        <v>20.271473085389466</v>
+        <f t="shared" ref="AA3:AA7" si="8">Y3-X3</f>
+        <v>41.285185477706683</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB5" si="9">X3-Z3</f>
-        <v>9.4803884781167831</v>
+        <f t="shared" ref="AB3:AB7" si="9">X3-Z3</f>
+        <v>24.01356642590887</v>
       </c>
       <c r="AD3">
         <f>(X3-$X$2)/ABS($X$2)*100</f>
-        <v>-42.83772333033081</v>
+        <v>-14.973286556239303</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>1920</v>
@@ -10354,16 +10418,16 @@
         <v>65536</v>
       </c>
       <c r="N4">
-        <v>40.042900000000003</v>
+        <v>30.0273</v>
       </c>
       <c r="O4">
-        <v>2182</v>
+        <v>1918</v>
       </c>
       <c r="P4">
-        <v>2.8689800000000001E-2</v>
+        <v>2.6415299999999999E-2</v>
       </c>
       <c r="Q4">
-        <v>9.5936000000000007E-3</v>
+        <v>9.2403999999999993E-3</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
@@ -10383,42 +10447,42 @@
       </c>
       <c r="W4">
         <f t="shared" si="4"/>
-        <v>1.8351466544454631E-2</v>
+        <v>1.5655526590198122E-2</v>
       </c>
       <c r="X4">
         <f t="shared" si="5"/>
-        <v>54.491557804254931</v>
+        <v>63.875206895058831</v>
       </c>
       <c r="Y4">
         <f t="shared" si="6"/>
-        <v>104.23615743829218</v>
+        <v>108.22042335829619</v>
       </c>
       <c r="Z4">
         <f t="shared" si="7"/>
-        <v>34.855593277053167</v>
+        <v>37.85684811453968</v>
       </c>
       <c r="AA4">
         <f t="shared" si="8"/>
-        <v>49.74459963403725</v>
+        <v>44.345216463237357</v>
       </c>
       <c r="AB4">
         <f t="shared" si="9"/>
-        <v>19.635964527201764</v>
+        <v>26.018358780519151</v>
       </c>
       <c r="AD4">
         <f>(X4-$X$2)/ABS($X$2)*100</f>
-        <v>-14.722203204850151</v>
+        <v>-0.22978344343498797</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>1920</v>
@@ -10451,16 +10515,16 @@
         <v>65536</v>
       </c>
       <c r="N5">
-        <v>40.046300000000002</v>
+        <v>30.084599999999998</v>
       </c>
       <c r="O5">
-        <v>1320</v>
+        <v>845</v>
       </c>
       <c r="P5">
-        <v>4.2053300000000002E-2</v>
+        <v>5.5558299999999998E-2</v>
       </c>
       <c r="Q5">
-        <v>1.8990900000000002E-2</v>
+        <v>2.0879399999999999E-2</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
@@ -10480,51 +10544,237 @@
       </c>
       <c r="W5">
         <f t="shared" si="4"/>
-        <v>3.0338106060606062E-2</v>
+        <v>3.5603076923076918E-2</v>
       </c>
       <c r="X5">
         <f t="shared" si="5"/>
-        <v>32.961846662488171</v>
+        <v>28.087460029383809</v>
       </c>
       <c r="Y5">
         <f t="shared" si="6"/>
-        <v>52.656798782574811</v>
+        <v>47.894096573656334</v>
       </c>
       <c r="Z5">
         <f t="shared" si="7"/>
-        <v>23.779346686229143</v>
+        <v>17.99911084392431</v>
       </c>
       <c r="AA5">
         <f t="shared" si="8"/>
-        <v>19.69495212008664</v>
+        <v>19.806636544272525</v>
       </c>
       <c r="AB5">
         <f t="shared" si="9"/>
-        <v>9.1824999762590274</v>
+        <v>10.088349185459499</v>
       </c>
       <c r="AD5">
         <f t="shared" ref="AD5:AD7" si="10">(X5-$X$2)/ABS($X$2)*100</f>
-        <v>-48.415611978392249</v>
+        <v>-56.128643555559862</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <v>1920</v>
+      </c>
+      <c r="E6">
+        <v>1080</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>256</v>
+      </c>
+      <c r="I6">
+        <v>1665</v>
+      </c>
+      <c r="J6">
+        <v>38</v>
+      </c>
+      <c r="K6">
+        <v>8589410304</v>
+      </c>
+      <c r="L6">
+        <v>49152</v>
+      </c>
+      <c r="M6">
+        <v>65536</v>
+      </c>
+      <c r="N6">
+        <v>30.075399999999998</v>
+      </c>
+      <c r="O6">
+        <v>781</v>
+      </c>
+      <c r="P6">
+        <v>6.1097899999999997E-2</v>
+      </c>
+      <c r="Q6">
+        <v>2.19572E-2</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>2073600</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" si="1"/>
+        <v>8.5894103039999994</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="2"/>
+        <v>49.152000000000001</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" si="3"/>
+        <v>65.536000000000001</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="4"/>
+        <v>3.8508834827144685E-2</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="5"/>
+        <v>25.968066925128181</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="6"/>
+        <v>45.543147578015414</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="7"/>
+        <v>16.367174649210529</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="8"/>
+        <v>19.575080652887234</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="9"/>
+        <v>9.6008922759176514</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="10"/>
+        <v>-59.439040801356199</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>1920</v>
+      </c>
+      <c r="E7">
+        <v>1080</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>256</v>
+      </c>
+      <c r="I7">
+        <v>1665</v>
+      </c>
+      <c r="J7">
+        <v>38</v>
+      </c>
+      <c r="K7">
+        <v>8589410304</v>
+      </c>
+      <c r="L7">
+        <v>49152</v>
+      </c>
+      <c r="M7">
+        <v>65536</v>
+      </c>
+      <c r="N7">
+        <v>30.083100000000002</v>
+      </c>
+      <c r="O7">
+        <v>777</v>
+      </c>
+      <c r="P7">
+        <v>6.1268700000000002E-2</v>
+      </c>
+      <c r="Q7">
+        <v>2.1770600000000001E-2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>2073600</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="1"/>
+        <v>8.5894103039999994</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="2"/>
+        <v>49.152000000000001</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" si="3"/>
+        <v>65.536000000000001</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="4"/>
+        <v>3.8716988416988417E-2</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="5"/>
+        <v>25.828455179153746</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="6"/>
+        <v>45.933506655765115</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="7"/>
+        <v>16.321547543851917</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="8"/>
+        <v>20.105051476611369</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="9"/>
+        <v>9.5069076353018289</v>
+      </c>
       <c r="AD7">
-        <f>SUM(AD3:AD4)</f>
-        <v>-57.559926535180963</v>
+        <f t="shared" si="10"/>
+        <v>-59.657108104881239</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AD9">
+        <f>SUM(AD3:AD7)</f>
+        <v>-190.42786246147162</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10536,7 +10786,7 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:AB6"/>
+      <selection activeCell="AB2" sqref="S2:AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10653,10 +10903,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>1920</v>
@@ -10746,10 +10996,10 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>1920</v>
@@ -10839,10 +11089,10 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1920</v>
@@ -10932,10 +11182,10 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>1920</v>
@@ -11025,10 +11275,10 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>1920</v>
@@ -11243,10 +11493,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>1920</v>
@@ -11333,13 +11583,13 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>1920</v>
@@ -11426,13 +11676,13 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>1920</v>
@@ -11522,10 +11772,10 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>1920</v>

</xml_diff>

<commit_message>
Added extra benchmark scene
</commit_message>
<xml_diff>
--- a/Deliverable 2/Results.xlsx
+++ b/Deliverable 2/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\dissertation\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746750AF-03A7-488D-A916-DEEF3C4443E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF16117-1C59-4ACF-9793-27E48FC4E794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="82">
   <si>
     <t>NVIDIA GeForce RTX 3060 Ti</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t xml:space="preserve">-cl-fast-relaxed-math -I "kernels" -I "kernels\benchmarks" -I "kernels\benchmarks\mandelbulb" -I "kernels\benchmarks\mandelbulb_stationary" -I "kernels\benchmarks\planet" -I "kernels\benchmarks\sierpinski" -I "kernels\benchmarks\spheres" -I "kernels\include" -I "kernels/include" </t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -4756,7 +4759,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Performance over Varying Resolutions</a:t>
+              <a:t>Mandelbulb Scene Performance for Varying Resolutions</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4832,6 +4835,256 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{568476AC-89E1-4B7C-9C19-69D3E68752B3}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A057C39E-84E0-4AD7-B85D-AACE3D934C4B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A2353463-13F2-408E-A2BD-759EF67D814C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BCDDF354-BE7A-40C1-AD20-0BFB48E0096C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{8546CFBA-576D-4E33-830D-51BE9C049FE2}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F73E1C7E-A068-439D-A7BE-EC329CF80CF2}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -4846,6 +5099,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.2144126394138621E-2"/>
+                  <c:y val="-1.7912909849999319E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4932,6 +5191,32 @@
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'Resolutions 3060TI'!$V$2:$V$7</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>1024x576</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1280x720</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1600x900</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1920x1080</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2560x1440</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3840x2160</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CB98-48A5-9FE0-B3D87D69B500}"/>
             </c:ext>
@@ -4973,6 +5258,256 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C152B0F0-C041-4AD7-BCE8-C1E3CF2BB174}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{68EF4B1B-0170-4A57-B34F-EB563A0AEF5A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BD72FCD1-F675-4EFF-9EE7-AF3AA36CDAA5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D377ABB6-401B-4D0F-9459-6E9BC2BEDF6D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2AB8D6DC-8693-4E5C-BEDB-FCBD28DC5A56}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FE26569A-25B2-417E-86AB-E8D04723E88D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -4987,6 +5522,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.4510290250985708E-2"/>
+                  <c:y val="-1.030013735329716E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5073,6 +5614,32 @@
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'Resolutions 1660TI'!$V$2:$V$7</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>1024x576</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1280x720</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1600x900</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1920x1080</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2560x1440</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3840x2160</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-722F-4C9E-80B3-79319AAA8A21}"/>
             </c:ext>
@@ -5114,6 +5681,256 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{162524D2-9AD1-4C83-959B-EB9802170EEE}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{14E7288F-DA85-4B89-995B-FDCD81B13A53}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5E91968D-0071-4627-A7EC-0231ADCF8768}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CCC3E30D-8FC7-4010-911F-3FC87BB7B498}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F90A12BB-8E67-496E-B658-4DE25938F6FD}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B6C7CD42-118F-4F17-83E8-9817BF3B2C7B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-4F8A-451F-B6A4-D0AD52F7F864}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -5128,6 +5945,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8547557331731048E-2"/>
+                  <c:y val="1.1285817252118097E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5214,6 +6037,32 @@
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'Resolutions 970 ME'!$V$2:$V$7</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>1024x576</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1280x720</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1600x900</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1920x1080</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2560x1440</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3840x2160</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-89E5-4AA9-9B65-FFCF79566B08}"/>
             </c:ext>
@@ -5221,7 +6070,7 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -11353,16 +12202,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>62193</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>45945</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>429185</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>160245</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11392,15 +12241,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>290232</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>37540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:colOff>366432</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>156603</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11695,8 +12544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668D4FD2-0EC3-4246-9368-74132FA6B2E6}">
   <dimension ref="AR24:AV28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN56" sqref="AN56"/>
+    <sheetView tabSelected="1" topLeftCell="P28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM42" sqref="AM42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12609,8 +13458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D811C00-07CB-4F03-B932-655B80B938E4}">
   <dimension ref="A1:AM19"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q19"/>
+    <sheetView topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12649,7 +13498,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -12751,6 +13600,10 @@
       <c r="AM1" s="6"/>
     </row>
     <row r="2" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(D2,"x",E2)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -12805,9 +13658,9 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="4" t="str">
         <f ca="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+        <v>1024x576</v>
       </c>
       <c r="W2">
         <f ca="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
@@ -12859,6 +13712,10 @@
       </c>
     </row>
     <row r="3" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A19" si="0">_xlfn.CONCAT(D3,"x",E3)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
@@ -12907,60 +13764,64 @@
       <c r="Q3">
         <v>9.1927999999999992E-3</v>
       </c>
-      <c r="V3" s="4">
-        <f t="shared" ref="V3:V7" ca="1" si="0">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+      <c r="V3" s="4" t="str">
+        <f t="shared" ref="V3:V7" ca="1" si="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
+        <v>1280x720</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W7" ca="1" si="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="W3:W7" ca="1" si="2">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
         <v>921600</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X7" ca="1" si="2">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="X3:X7" ca="1" si="3">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
         <v>38</v>
       </c>
       <c r="Y3" s="3">
-        <f t="shared" ref="Y3:Y7" si="3">K3/1000000000</f>
+        <f t="shared" ref="Y3:Y7" si="4">K3/1000000000</f>
         <v>8.5894103039999994</v>
       </c>
       <c r="Z3" s="3">
-        <f t="shared" ref="Z3:Z7" si="4">L3/1000</f>
+        <f t="shared" ref="Z3:Z7" si="5">L3/1000</f>
         <v>49.152000000000001</v>
       </c>
       <c r="AA3" s="3">
-        <f t="shared" ref="AA3:AA7" si="5">M3/1000</f>
+        <f t="shared" ref="AA3:AA7" si="6">M3/1000</f>
         <v>65.536000000000001</v>
       </c>
       <c r="AB3" s="4">
-        <f t="shared" ref="AB3:AB7" ca="1" si="6">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AB3:AB7" ca="1" si="7">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
         <v>90.146900000000002</v>
       </c>
       <c r="AC3" s="4">
-        <f t="shared" ref="AC3:AC7" ca="1" si="7">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AC3:AC7" ca="1" si="8">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
         <v>4019</v>
       </c>
       <c r="AD3" s="4">
-        <f t="shared" ref="AD3:AD7" ca="1" si="8">AC3/AB3</f>
+        <f t="shared" ref="AD3:AD7" ca="1" si="9">AC3/AB3</f>
         <v>44.58278654063534</v>
       </c>
       <c r="AE3" s="4">
-        <f t="shared" ref="AE3:AE7" ca="1" si="9">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AE3:AE7" ca="1" si="10">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
         <v>78.37850547865753</v>
       </c>
       <c r="AF3" s="4">
-        <f t="shared" ref="AF3:AF7" ca="1" si="10">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AF3:AF7" ca="1" si="11">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
         <v>28.636064259328197</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG7" ca="1" si="11">AE3-AD3</f>
+        <f t="shared" ref="AG3:AG7" ca="1" si="12">AE3-AD3</f>
         <v>33.795718938022191</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH7" ca="1" si="12">AE3-AF3</f>
+        <f t="shared" ref="AH3:AH7" ca="1" si="13">AE3-AF3</f>
         <v>49.742441219329336</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>1024x576</v>
+      </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
@@ -13009,60 +13870,64 @@
       <c r="Q4">
         <v>9.5145999999999998E-3</v>
       </c>
-      <c r="V4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V4" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1600x900</v>
       </c>
       <c r="W4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1440000</v>
       </c>
       <c r="X4">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
       <c r="Y4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5894103039999994</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA4" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB4" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>90.149499999999989</v>
       </c>
       <c r="AC4" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>2943</v>
       </c>
       <c r="AD4" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>32.645771745822223</v>
       </c>
       <c r="AE4" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>57.495055425233431</v>
       </c>
       <c r="AF4" s="4">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>19.815988728665612</v>
       </c>
       <c r="AG4">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>24.849283679411208</v>
       </c>
       <c r="AH4">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>37.679066696567816</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -13111,60 +13976,64 @@
       <c r="Q5">
         <v>1.25728E-2</v>
       </c>
-      <c r="V5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V5" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1920x1080</v>
       </c>
       <c r="W5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2073600</v>
       </c>
       <c r="X5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
       <c r="Y5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5894103039999994</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB5" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>90.244</v>
       </c>
       <c r="AC5" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>2297</v>
       </c>
       <c r="AD5" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>25.453215726253269</v>
       </c>
       <c r="AE5" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>45.128390270319052</v>
       </c>
       <c r="AF5" s="4">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>15.861535142817264</v>
       </c>
       <c r="AG5">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>19.675174544065783</v>
       </c>
       <c r="AH5">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>29.266855127501788</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -13213,60 +14082,64 @@
       <c r="Q6">
         <v>1.25732E-2</v>
       </c>
-      <c r="V6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V6" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2560x1440</v>
       </c>
       <c r="W6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3686400</v>
       </c>
       <c r="X6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
       <c r="Y6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5894103039999994</v>
       </c>
       <c r="Z6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB6" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>90.482900000000001</v>
       </c>
       <c r="AC6" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>1517</v>
       </c>
       <c r="AD6" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>16.765598803751868</v>
       </c>
       <c r="AE6" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>30.171919597868651</v>
       </c>
       <c r="AF6" s="4">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>10.137135164505429</v>
       </c>
       <c r="AG6">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>13.406320794116784</v>
       </c>
       <c r="AH6">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>20.034784433363221</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -13317,60 +14190,64 @@
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-      <c r="V7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V7" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3840x2160</v>
       </c>
       <c r="W7">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8294400</v>
       </c>
       <c r="X7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
       <c r="Y7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5894103039999994</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB7" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>90.739699999999999</v>
       </c>
       <c r="AC7" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>828</v>
       </c>
       <c r="AD7" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>9.1250026173769587</v>
       </c>
       <c r="AE7" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>16.152009794578738</v>
       </c>
       <c r="AF7" s="4">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>5.4994308089112778</v>
       </c>
       <c r="AG7">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>7.0270071772017797</v>
       </c>
       <c r="AH7">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>10.652578985667461</v>
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
@@ -13432,6 +14309,10 @@
       <c r="AF8" s="4"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -13493,6 +14374,10 @@
       <c r="AF9" s="4"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B10" t="s">
         <v>38</v>
       </c>
@@ -13554,6 +14439,10 @@
       <c r="AF10" s="4"/>
     </row>
     <row r="11" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -13612,6 +14501,10 @@
       <c r="AF11" s="4"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -13670,6 +14563,10 @@
       <c r="AF12" s="4"/>
     </row>
     <row r="13" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -13728,6 +14625,10 @@
       <c r="AF13" s="4"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -13778,6 +14679,10 @@
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -13828,6 +14733,10 @@
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -13877,7 +14786,11 @@
         <v>3.3143400000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -13927,7 +14840,11 @@
         <v>6.1911800000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -13977,7 +14894,11 @@
         <v>6.1569199999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
@@ -14037,8 +14958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FDBFBA-A177-4A15-AAD1-5E104CD34D5D}">
   <dimension ref="A1:AM19"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14077,7 +14998,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -14179,6 +15100,10 @@
       <c r="AM1" s="6"/>
     </row>
     <row r="2" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(D2,"x",E2)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -14233,9 +15158,9 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="4" t="str">
         <f ca="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+        <v>1024x576</v>
       </c>
       <c r="W2">
         <f ca="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
@@ -14287,6 +15212,10 @@
       </c>
     </row>
     <row r="3" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A19" si="0">_xlfn.CONCAT(D3,"x",E3)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
@@ -14335,60 +15264,64 @@
       <c r="Q3">
         <v>1.8602199999999999E-2</v>
       </c>
-      <c r="V3" s="4">
-        <f t="shared" ref="V3:V7" ca="1" si="0">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+      <c r="V3" s="4" t="str">
+        <f t="shared" ref="V3:V7" ca="1" si="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
+        <v>1280x720</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W7" ca="1" si="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="W3:W7" ca="1" si="2">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
         <v>921600</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X7" ca="1" si="2">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="X3:X7" ca="1" si="3">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
         <v>24</v>
       </c>
       <c r="Y3" s="3">
-        <f t="shared" ref="Y3:Y7" si="3">K3/1000000000</f>
+        <f t="shared" ref="Y3:Y7" si="4">K3/1000000000</f>
         <v>6.4419921919999998</v>
       </c>
       <c r="Z3" s="3">
-        <f t="shared" ref="Z3:AA7" si="4">L3/1000</f>
+        <f t="shared" ref="Z3:AA7" si="5">L3/1000</f>
         <v>49.152000000000001</v>
       </c>
       <c r="AA3" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB3" s="4">
-        <f t="shared" ref="AB3:AB7" ca="1" si="5">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AB3:AB7" ca="1" si="6">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
         <v>90.474599999999995</v>
       </c>
       <c r="AC3" s="4">
-        <f t="shared" ref="AC3:AC7" ca="1" si="6">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AC3:AC7" ca="1" si="7">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
         <v>1758</v>
       </c>
       <c r="AD3" s="4">
-        <f t="shared" ref="AD3:AD7" ca="1" si="7">AC3/AB3</f>
+        <f t="shared" ref="AD3:AD7" ca="1" si="8">AC3/AB3</f>
         <v>19.430867889993436</v>
       </c>
       <c r="AE3" s="4">
-        <f t="shared" ref="AE3:AE7" ca="1" si="8">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AE3:AE7" ca="1" si="9">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
         <v>37.858997948042308</v>
       </c>
       <c r="AF3" s="4">
-        <f t="shared" ref="AF3:AF7" ca="1" si="9">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AF3:AF7" ca="1" si="10">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
         <v>10.208946508182981</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG7" ca="1" si="10">AE3-AD3</f>
+        <f t="shared" ref="AG3:AG7" ca="1" si="11">AE3-AD3</f>
         <v>18.428130058048872</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH7" ca="1" si="11">AE3-AF3</f>
+        <f t="shared" ref="AH3:AH7" ca="1" si="12">AE3-AF3</f>
         <v>27.650051439859325</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>1024x576</v>
+      </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
@@ -14437,60 +15370,64 @@
       <c r="Q4">
         <v>1.8528200000000002E-2</v>
       </c>
-      <c r="V4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V4" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1600x900</v>
       </c>
       <c r="W4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1440000</v>
       </c>
       <c r="X4">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>24</v>
       </c>
       <c r="Y4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.4419921919999998</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB4" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>90.594099999999997</v>
       </c>
       <c r="AC4" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>1239</v>
       </c>
       <c r="AD4" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>13.676387314405684</v>
       </c>
       <c r="AE4" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>26.620595289751872</v>
       </c>
       <c r="AF4" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>7.0163129275565685</v>
       </c>
       <c r="AG4">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>12.944207975346188</v>
       </c>
       <c r="AH4">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>19.604282362195303</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -14539,60 +15476,64 @@
       <c r="Q5">
         <v>2.63871E-2</v>
       </c>
-      <c r="V5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V5" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1920x1080</v>
       </c>
       <c r="W5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2073600</v>
       </c>
       <c r="X5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>24</v>
       </c>
       <c r="Y5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.4419921919999998</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB5" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>90.88</v>
       </c>
       <c r="AC5" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>941</v>
       </c>
       <c r="AD5" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>10.35431338028169</v>
       </c>
       <c r="AE5" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>20.207613016127699</v>
       </c>
       <c r="AF5" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>5.3266288831124564</v>
       </c>
       <c r="AG5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>9.8532996358460085</v>
       </c>
       <c r="AH5">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>14.880984133015243</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -14641,60 +15582,64 @@
       <c r="Q6">
         <v>2.6413800000000001E-2</v>
       </c>
-      <c r="V6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V6" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2560x1440</v>
       </c>
       <c r="W6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3686400</v>
       </c>
       <c r="X6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>24</v>
       </c>
       <c r="Y6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.4419921919999998</v>
       </c>
       <c r="Z6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB6" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>90.966399999999993</v>
       </c>
       <c r="AC6" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>606</v>
       </c>
       <c r="AD6" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.6618004010271932</v>
       </c>
       <c r="AE6" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>13.114650901107662</v>
       </c>
       <c r="AF6" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>3.3799427437699205</v>
       </c>
       <c r="AG6">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6.4528505000804692</v>
       </c>
       <c r="AH6">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>9.7347081573377423</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -14745,60 +15690,64 @@
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-      <c r="V7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V7" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3840x2160</v>
       </c>
       <c r="W7">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8294400</v>
       </c>
       <c r="X7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>24</v>
       </c>
       <c r="Y7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.4419921919999998</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB7" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>92.538600000000002</v>
       </c>
       <c r="AC7" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>331</v>
       </c>
       <c r="AD7" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3.5768857536206511</v>
       </c>
       <c r="AE7" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>7.0675873377105258</v>
       </c>
       <c r="AF7" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1.8161048546298868</v>
       </c>
       <c r="AG7">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>3.4907015840898747</v>
       </c>
       <c r="AH7">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>5.2514824830806388</v>
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
@@ -14860,6 +15809,10 @@
       <c r="AF8" s="4"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -14921,6 +15874,10 @@
       <c r="AF9" s="4"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B10" t="s">
         <v>38</v>
       </c>
@@ -14982,6 +15939,10 @@
       <c r="AF10" s="4"/>
     </row>
     <row r="11" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -15040,6 +16001,10 @@
       <c r="AF11" s="4"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -15098,6 +16063,10 @@
       <c r="AF12" s="4"/>
     </row>
     <row r="13" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -15156,6 +16125,10 @@
       <c r="AF13" s="4"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -15206,6 +16179,10 @@
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -15256,6 +16233,10 @@
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -15305,7 +16286,11 @@
         <v>7.6250600000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -15355,7 +16340,11 @@
         <v>0.14074400000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -15405,7 +16394,11 @@
         <v>0.14138200000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
@@ -15465,8 +16458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34151026-92BE-4E45-B64A-8BFC36898D47}">
   <dimension ref="A1:AM19"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q19"/>
+    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15505,7 +16498,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -15607,6 +16600,10 @@
       <c r="AM1" s="6"/>
     </row>
     <row r="2" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(D2,"x",E2)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -15661,9 +16658,9 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="4" t="str">
         <f ca="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+        <v>1024x576</v>
       </c>
       <c r="W2">
         <f ca="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
@@ -15715,6 +16712,10 @@
       </c>
     </row>
     <row r="3" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A19" si="0">_xlfn.CONCAT(D3,"x",E3)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
@@ -15763,60 +16764,64 @@
       <c r="Q3">
         <v>3.4477899999999999E-2</v>
       </c>
-      <c r="V3" s="4">
-        <f t="shared" ref="V3:V7" ca="1" si="0">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+      <c r="V3" s="4" t="str">
+        <f t="shared" ref="V3:V7" ca="1" si="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
+        <v>1280x720</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W7" ca="1" si="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="W3:W7" ca="1" si="2">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
         <v>921600</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X7" ca="1" si="2">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="X3:X7" ca="1" si="3">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
         <v>13</v>
       </c>
       <c r="Y3" s="3">
-        <f t="shared" ref="Y3:Y7" si="3">K3/1000000000</f>
+        <f t="shared" ref="Y3:Y7" si="4">K3/1000000000</f>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z3" s="3">
-        <f t="shared" ref="Z3:AA7" si="4">L3/1000</f>
+        <f t="shared" ref="Z3:AA7" si="5">L3/1000</f>
         <v>49.152000000000001</v>
       </c>
       <c r="AA3" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB3" s="4">
-        <f t="shared" ref="AB3:AB7" ca="1" si="5">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AB3:AB7" ca="1" si="6">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
         <v>91.046499999999995</v>
       </c>
       <c r="AC3" s="4">
-        <f t="shared" ref="AC3:AC7" ca="1" si="6">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AC3:AC7" ca="1" si="7">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
         <v>843</v>
       </c>
       <c r="AD3" s="4">
-        <f t="shared" ref="AD3:AD7" ca="1" si="7">AC3/AB3</f>
+        <f t="shared" ref="AD3:AD7" ca="1" si="8">AC3/AB3</f>
         <v>9.2590050139214579</v>
       </c>
       <c r="AE3" s="4">
-        <f t="shared" ref="AE3:AE7" ca="1" si="8">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AE3:AE7" ca="1" si="9">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
         <v>20.31719200152785</v>
       </c>
       <c r="AF3" s="4">
-        <f t="shared" ref="AF3:AF7" ca="1" si="9">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AF3:AF7" ca="1" si="10">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
         <v>3.1257032832387286</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG7" ca="1" si="10">AE3-AD3</f>
+        <f t="shared" ref="AG3:AG7" ca="1" si="11">AE3-AD3</f>
         <v>11.058186987606392</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH7" ca="1" si="11">AE3-AF3</f>
+        <f t="shared" ref="AH3:AH7" ca="1" si="12">AE3-AF3</f>
         <v>17.191488718289122</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>1024x576</v>
+      </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
@@ -15865,60 +16870,64 @@
       <c r="Q4">
         <v>3.4729299999999998E-2</v>
       </c>
-      <c r="V4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V4" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1600x900</v>
       </c>
       <c r="W4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1440000</v>
       </c>
       <c r="X4">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB4" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>91.952100000000002</v>
       </c>
       <c r="AC4" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>601</v>
       </c>
       <c r="AD4" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.5360116843443485</v>
       </c>
       <c r="AE4" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>14.12048444558036</v>
       </c>
       <c r="AF4" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>2.1462359314234694</v>
       </c>
       <c r="AG4">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>7.584472761236011</v>
       </c>
       <c r="AH4">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>11.974248514156891</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -15967,60 +16976,64 @@
       <c r="Q5">
         <v>4.9219400000000003E-2</v>
       </c>
-      <c r="V5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V5" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1920x1080</v>
       </c>
       <c r="W5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2073600</v>
       </c>
       <c r="X5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB5" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>92.967199999999991</v>
       </c>
       <c r="AC5" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>461</v>
       </c>
       <c r="AD5" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>4.9587381356005134</v>
       </c>
       <c r="AE5" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>10.639452366107811</v>
       </c>
       <c r="AF5" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1.6118217454095318</v>
       </c>
       <c r="AG5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>5.6807142305072977</v>
       </c>
       <c r="AH5">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>9.0276306206982788</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -16069,60 +17082,64 @@
       <c r="Q6">
         <v>4.9014599999999998E-2</v>
       </c>
-      <c r="V6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V6" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2560x1440</v>
       </c>
       <c r="W6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3686400</v>
       </c>
       <c r="X6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB6" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>95.537399999999991</v>
       </c>
       <c r="AC6" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>306</v>
       </c>
       <c r="AD6" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3.2029341388817367</v>
       </c>
       <c r="AE6" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>6.8243547572577015</v>
       </c>
       <c r="AF6" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1.0508396208570647</v>
       </c>
       <c r="AG6">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>3.6214206183759647</v>
       </c>
       <c r="AH6">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>5.7735151364006363</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -16173,60 +17190,64 @@
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-      <c r="V7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V7" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3840x2160</v>
       </c>
       <c r="W7">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8294400</v>
       </c>
       <c r="X7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB7" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>94.522799999999989</v>
       </c>
       <c r="AC7" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>177</v>
       </c>
       <c r="AD7" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>1.8725640797775778</v>
       </c>
       <c r="AE7" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>3.6806925591119226</v>
       </c>
       <c r="AF7" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0.9867966606801003</v>
       </c>
       <c r="AG7">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>1.8081284793343448</v>
       </c>
       <c r="AH7">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>2.6938958984318222</v>
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
@@ -16288,6 +17309,10 @@
       <c r="AF8" s="4"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -16349,6 +17374,10 @@
       <c r="AF9" s="4"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B10" t="s">
         <v>38</v>
       </c>
@@ -16410,6 +17439,10 @@
       <c r="AF10" s="4"/>
     </row>
     <row r="11" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -16468,6 +17501,10 @@
       <c r="AF11" s="4"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -16526,6 +17563,10 @@
       <c r="AF12" s="4"/>
     </row>
     <row r="13" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -16584,6 +17625,10 @@
       <c r="AF13" s="4"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -16634,6 +17679,10 @@
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -16684,6 +17733,10 @@
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -16733,7 +17786,11 @@
         <v>0.146534</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -16783,7 +17840,11 @@
         <v>0.27085799999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -16833,7 +17894,11 @@
         <v>0.27144699999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
@@ -16893,8 +17958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A257A558-688E-43F1-9D27-FDF623F82362}">
   <dimension ref="A1:AM19"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16933,7 +17998,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -17035,6 +18100,10 @@
       <c r="AM1" s="6"/>
     </row>
     <row r="2" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(D2,"x",E2)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -17089,9 +18158,9 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="4" t="str">
         <f ca="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+        <v>1024x576</v>
       </c>
       <c r="W2">
         <f ca="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
@@ -17143,6 +18212,10 @@
       </c>
     </row>
     <row r="3" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A19" si="0">_xlfn.CONCAT(D3,"x",E3)</f>
+        <v>1024x576</v>
+      </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
@@ -17191,60 +18264,64 @@
       <c r="Q3">
         <v>3.2557799999999998E-2</v>
       </c>
-      <c r="V3" s="4">
-        <f t="shared" ref="V3:V7" ca="1" si="0">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
-        <v>0</v>
+      <c r="V3" s="4" t="str">
+        <f t="shared" ref="V3:V7" ca="1" si="1">INDEX(OFFSET($A$2,(ROW()-ROW($V$2))*$S$2,,$S$2,),1)</f>
+        <v>1280x720</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W7" ca="1" si="1">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="W3:W7" ca="1" si="2">OFFSET($D$1,(ROW()-1)*$S$2,0) * OFFSET($E$1,(ROW()-1)*$S$2,0)</f>
         <v>921600</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X7" ca="1" si="2">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
+        <f t="shared" ref="X3:X7" ca="1" si="3">OFFSET($J$1,(ROW()-1)*$S$2,0)</f>
         <v>13</v>
       </c>
       <c r="Y3" s="3">
-        <f t="shared" ref="Y3:Y7" si="3">K3/1000000000</f>
+        <f t="shared" ref="Y3:Y7" si="4">K3/1000000000</f>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z3" s="3">
-        <f t="shared" ref="Z3:AA7" si="4">L3/1000</f>
+        <f t="shared" ref="Z3:AA7" si="5">L3/1000</f>
         <v>49.152000000000001</v>
       </c>
       <c r="AA3" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB3" s="4">
-        <f t="shared" ref="AB3:AB7" ca="1" si="5">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AB3:AB7" ca="1" si="6">SUM(OFFSET($N$2,(ROW()-ROW($AB$2))*$S$2,,$S$2,))</f>
         <v>90.828299999999999</v>
       </c>
       <c r="AC3" s="4">
-        <f t="shared" ref="AC3:AC7" ca="1" si="6">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AC3:AC7" ca="1" si="7">SUM(OFFSET($O$2,(ROW()-ROW($AC$2))*$S$2,,$S$2,))</f>
         <v>983</v>
       </c>
       <c r="AD3" s="4">
-        <f t="shared" ref="AD3:AD7" ca="1" si="7">AC3/AB3</f>
+        <f t="shared" ref="AD3:AD7" ca="1" si="8">AC3/AB3</f>
         <v>10.822618060670518</v>
       </c>
       <c r="AE3" s="4">
-        <f t="shared" ref="AE3:AE7" ca="1" si="8">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AE3:AE7" ca="1" si="9">1/MAX(OFFSET($Q$2,(ROW()-ROW($AE$2))*$S$2,,$S$2,))</f>
         <v>21.540907259931974</v>
       </c>
       <c r="AF3" s="4">
-        <f t="shared" ref="AF3:AF7" ca="1" si="9">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
+        <f t="shared" ref="AF3:AF7" ca="1" si="10">1/MIN(OFFSET($P$2,(ROW()-ROW($AF$2))*$S$2,,$S$2,))</f>
         <v>5.737596750225201</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG7" ca="1" si="10">AE3-AD3</f>
+        <f t="shared" ref="AG3:AG7" ca="1" si="11">AE3-AD3</f>
         <v>10.718289199261456</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH7" ca="1" si="11">AE3-AF3</f>
+        <f t="shared" ref="AH3:AH7" ca="1" si="12">AE3-AF3</f>
         <v>15.803310509706773</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>1024x576</v>
+      </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
@@ -17293,60 +18370,64 @@
       <c r="Q4">
         <v>3.2745099999999999E-2</v>
       </c>
-      <c r="V4" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V4" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1600x900</v>
       </c>
       <c r="W4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1440000</v>
       </c>
       <c r="X4">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB4" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>91.203800000000001</v>
       </c>
       <c r="AC4" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>690</v>
       </c>
       <c r="AD4" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.5654742455906439</v>
       </c>
       <c r="AE4" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>15.094954813252768</v>
       </c>
       <c r="AF4" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>3.9262955793838072</v>
       </c>
       <c r="AG4">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>7.5294805676621239</v>
       </c>
       <c r="AH4">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>11.168659233868961</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -17395,60 +18476,64 @@
       <c r="Q5">
         <v>4.60531E-2</v>
       </c>
-      <c r="V5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V5" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>1920x1080</v>
       </c>
       <c r="W5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2073600</v>
       </c>
       <c r="X5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB5" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>91.49799999999999</v>
       </c>
       <c r="AC5" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>522</v>
       </c>
       <c r="AD5" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>5.705042733174496</v>
       </c>
       <c r="AE5" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>11.481398985503585</v>
       </c>
       <c r="AF5" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>2.9662412088026171</v>
       </c>
       <c r="AG5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>5.776356252329089</v>
       </c>
       <c r="AH5">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>8.515157776700967</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -17497,60 +18582,64 @@
       <c r="Q6">
         <v>4.6423300000000001E-2</v>
       </c>
-      <c r="V6" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V6" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2560x1440</v>
       </c>
       <c r="W6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>3686400</v>
       </c>
       <c r="X6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB6" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>91.784800000000004</v>
       </c>
       <c r="AC6" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>336</v>
       </c>
       <c r="AD6" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3.6607368540324758</v>
       </c>
       <c r="AE6" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>7.3815991496397775</v>
       </c>
       <c r="AF6" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1.8786857465991094</v>
       </c>
       <c r="AG6">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>3.7208622956073016</v>
       </c>
       <c r="AH6">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>5.5029134030406679</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>1280x720</v>
+      </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -17601,60 +18690,64 @@
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-      <c r="V7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+      <c r="V7" s="4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3840x2160</v>
       </c>
       <c r="W7">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8294400</v>
       </c>
       <c r="X7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
       <c r="Y7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2947051519999997</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49.152000000000001</v>
       </c>
       <c r="AA7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.536000000000001</v>
       </c>
       <c r="AB7" s="4">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>97.433499999999995</v>
       </c>
       <c r="AC7" s="4">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>181</v>
       </c>
       <c r="AD7" s="4">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>1.857677287585892</v>
       </c>
       <c r="AE7" s="4">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>3.995189791491045</v>
       </c>
       <c r="AF7" s="4">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0.50941137515600721</v>
       </c>
       <c r="AG7">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2.1375125039051532</v>
       </c>
       <c r="AH7">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>3.4857784163350378</v>
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
@@ -17716,6 +18809,10 @@
       <c r="AF8" s="4"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -17777,6 +18874,10 @@
       <c r="AF9" s="4"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>1600x900</v>
+      </c>
       <c r="B10" t="s">
         <v>38</v>
       </c>
@@ -17838,6 +18939,10 @@
       <c r="AF10" s="4"/>
     </row>
     <row r="11" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -17896,6 +19001,10 @@
       <c r="AF11" s="4"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -17954,6 +19063,10 @@
       <c r="AF12" s="4"/>
     </row>
     <row r="13" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>1920x1080</v>
+      </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -18012,6 +19125,10 @@
       <c r="AF13" s="4"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -18062,6 +19179,10 @@
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -18112,6 +19233,10 @@
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>2560x1440</v>
+      </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -18161,7 +19286,11 @@
         <v>0.13547200000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -18211,7 +19340,11 @@
         <v>0.249779</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -18261,7 +19394,11 @@
         <v>0.25001000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>3840x2160</v>
+      </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Report and documentation update
</commit_message>
<xml_diff>
--- a/Deliverable 2/Results.xlsx
+++ b/Deliverable 2/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\dissertation\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79197FD-04EC-491B-ABAB-B20AEBDB1431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A3CF1F-EA97-4194-990C-740279602AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="801" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="801" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="2" r:id="rId1"/>
@@ -1186,7 +1186,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{46E3C727-8DB6-4031-973C-B970CB4BEF3B}" type="CELLRANGE">
+                    <a:fld id="{E1238542-CC76-41F9-AE16-E3B89C1DDB50}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1220,7 +1220,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38F4FE83-F47E-4D56-8CBC-B7363DBF74C2}" type="CELLRANGE">
+                    <a:fld id="{AE585E39-E95D-43E2-B859-88E24D9122CC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1254,7 +1254,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A3D0F21-4514-4B2A-A7F4-460354291A73}" type="CELLRANGE">
+                    <a:fld id="{5BE78C99-B719-40D1-9742-56E243C50B4D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1288,7 +1288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C286C13-FE2F-44B3-9165-574CEFEBCBA6}" type="CELLRANGE">
+                    <a:fld id="{329FA1B9-A9E7-4FA9-9176-AE35F6C89040}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1322,7 +1322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B7DE170-1835-475B-9D6A-E46031340343}" type="CELLRANGE">
+                    <a:fld id="{6C36850F-2773-436E-BF61-83025CAA6950}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2698,7 +2698,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3297124-74F4-4911-A9AA-1E8100BFA1C1}" type="CELLRANGE">
+                    <a:fld id="{3411C5B5-1990-4E46-9A4C-179C8118706A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2732,7 +2732,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3317872-102B-44FF-9460-ECD585F94010}" type="CELLRANGE">
+                    <a:fld id="{9CCC6CAF-CC90-47FF-9C2A-75CE7F15D21C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2766,7 +2766,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{257C4019-C1E3-47E3-A7FD-A85F8472A2A7}" type="CELLRANGE">
+                    <a:fld id="{0A503035-CD49-4E80-9B01-349ABA62FC26}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2800,7 +2800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{004A0D5F-97B9-4A8F-A6B1-DC57BF6C4738}" type="CELLRANGE">
+                    <a:fld id="{4D10EF15-2569-4CF7-AB62-B7E09F80AA80}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2834,7 +2834,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD611D06-BFEA-4880-94D9-E5CB7C74DF7B}" type="CELLRANGE">
+                    <a:fld id="{2AE0D466-5058-4FB6-9D13-BD2B74179784}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4304,7 +4304,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BC0168C-3A87-4A4A-BA2E-4A78335394C1}" type="CELLRANGE">
+                    <a:fld id="{F6A9A02D-7DDA-448F-8D6E-C5559619F76E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4338,7 +4338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C3336E4-E703-4593-9306-0149AD95A62A}" type="CELLRANGE">
+                    <a:fld id="{1D921954-F667-43F8-88B3-65386CF7D090}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4372,7 +4372,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA668BF6-A6C4-442E-BFE5-57EF4A190D26}" type="CELLRANGE">
+                    <a:fld id="{AD13DD27-7552-4242-AA63-B2A78C2FC595}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4406,7 +4406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79762663-F2C0-4FEA-890E-5F2F588877D7}" type="CELLRANGE">
+                    <a:fld id="{8E03ED03-DA42-48E1-86E1-FA1D7E39E3BE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4440,7 +4440,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D68B8F59-1FEB-4D9B-A530-E3DD0F20E820}" type="CELLRANGE">
+                    <a:fld id="{EDEDEB78-B625-4189-B4CB-5BC99B8ADA51}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5816,7 +5816,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32B1B37B-1917-4690-B300-862EDF4B5676}" type="CELLRANGE">
+                    <a:fld id="{4B61BDE1-A6BE-4E94-895F-4EBF6549C19A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5850,7 +5850,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F23BD6F-5D9E-4444-B2E1-403EFF04B383}" type="CELLRANGE">
+                    <a:fld id="{F9E44FFF-2F12-4725-A753-C1277AA29BD8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5884,7 +5884,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D4BCCD8-C3CF-45A9-B847-DAB55C5531E8}" type="CELLRANGE">
+                    <a:fld id="{3E2E1E67-F012-4540-A59B-E4F0EB95C0EC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5918,7 +5918,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3E739D9-ECA1-4939-9EC8-E470FB5DD049}" type="CELLRANGE">
+                    <a:fld id="{F617BB5D-AB2E-4924-9712-C6B2A0A867B7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5952,7 +5952,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E54020B-41AB-4348-8383-F3830FA6A279}" type="CELLRANGE">
+                    <a:fld id="{E8CBD1B8-241C-4A8C-B193-5D5814FC6907}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6639,7 +6639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00A60F10-7DFB-48C9-963D-8E1F36C7808B}" type="CELLRANGE">
+                    <a:fld id="{65B09EF7-CB08-4CF7-BF8C-665B7D7E6187}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6673,7 +6673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF54EF38-0657-43AA-8F1F-3221D482C292}" type="CELLRANGE">
+                    <a:fld id="{3B0146C9-ED74-4C83-8A86-953B89956EDC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6707,7 +6707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAADC8BD-2E7A-4AFF-AF25-8DB9DC38438A}" type="CELLRANGE">
+                    <a:fld id="{BFCA45AD-A716-4D57-833F-BB22B23CB3F0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6741,7 +6741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{46E4E3F7-AC55-44C4-A056-263C903587AA}" type="CELLRANGE">
+                    <a:fld id="{22D9570E-54D4-4961-A491-1E93D223851D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6775,7 +6775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCED2DC4-C354-4655-A92D-7B2D2E987493}" type="CELLRANGE">
+                    <a:fld id="{3CE5B90B-649B-4E2C-8B80-44C2261A7840}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8151,7 +8151,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC41548F-B39C-4978-903F-EFA8CF212B4B}" type="CELLRANGE">
+                    <a:fld id="{A202A827-EE50-41E0-9C8B-FC7E62D5DE81}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8185,7 +8185,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1089E29F-5C68-4F9B-A7AA-12821B7C0886}" type="CELLRANGE">
+                    <a:fld id="{48EEFD90-A137-4B6E-9B40-72EF360D8011}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8219,7 +8219,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E84A3DC6-9A2B-45CE-9A70-1314499F53EE}" type="CELLRANGE">
+                    <a:fld id="{37AC4F23-04D7-47F8-9739-498A07BC483B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8253,7 +8253,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E57FE33-F4D0-4851-ACDE-19A723B2CC83}" type="CELLRANGE">
+                    <a:fld id="{2862BBB0-1679-4888-AAB2-AA47E7B56DCC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8287,7 +8287,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7913B0D6-AECF-44FD-B1A0-4B7F8EE5E64D}" type="CELLRANGE">
+                    <a:fld id="{6E1B9767-BDAA-42A2-BFFD-2DB8D177D213}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9322,7 +9322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B09497F-2E6F-439E-BD85-D83DF097090D}" type="CELLRANGE">
+                    <a:fld id="{BB2A9CA5-5BC8-4E08-8E0C-A8B7DD77C8C7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9356,7 +9356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82AFA958-A121-426F-8123-472103503D0C}" type="CELLRANGE">
+                    <a:fld id="{FD6B7DE5-A68D-48E2-8944-43B08964053F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9390,7 +9390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D5E1AE7-056E-4507-8B84-B4B368501BAE}" type="CELLRANGE">
+                    <a:fld id="{9E46D2F1-30A9-48E0-AC98-3D2EA096D8FA}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9424,7 +9424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{349EED72-CB0B-4BBD-B2B6-F795EC9A3583}" type="CELLRANGE">
+                    <a:fld id="{49497E25-6611-46F7-8F3A-93192793F1C0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9458,7 +9458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1249E2D5-4E3B-43CF-92FA-F9EDFE4A1167}" type="CELLRANGE">
+                    <a:fld id="{ACFA4736-59F0-4039-9B85-EED6B9268D93}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10145,7 +10145,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EFB949F-102A-463D-8E88-33A3DE91518E}" type="CELLRANGE">
+                    <a:fld id="{1AD245A7-991C-4C5E-8514-2C86364B3FAD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10179,7 +10179,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62DE5D35-9E3F-4854-98F3-2966690278CE}" type="CELLRANGE">
+                    <a:fld id="{FAEA9915-5F56-4BBD-89CA-F490043418BC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10213,7 +10213,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDD4B2FA-3F9F-40F4-A437-1FF151270380}" type="CELLRANGE">
+                    <a:fld id="{76E468F9-6ED7-4441-A4B5-8942F14EADD5}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10247,7 +10247,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F164C78-28CF-4893-98CF-4445173FD381}" type="CELLRANGE">
+                    <a:fld id="{64E4761F-3A30-4C1C-B2E0-8B5CAB374397}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10281,7 +10281,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{947741C2-2F5F-4B2F-97F8-39CC98933B0B}" type="CELLRANGE">
+                    <a:fld id="{035016D3-A928-411A-BE0B-01AF304B0A02}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13003,7 +13003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6E2983A-310A-42C9-AD8A-53917352A8D0}" type="CELLRANGE">
+                    <a:fld id="{0F89ECD2-B03A-4EEB-99E5-679EE9DDF77D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13037,7 +13037,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BAAF229-28BE-4DD0-9484-251C007698C6}" type="CELLRANGE">
+                    <a:fld id="{E7BC44F7-DE0E-4D8C-9785-060141C21B45}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13071,7 +13071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{079D573F-B020-4CD9-8EBA-794C72E189DD}" type="CELLRANGE">
+                    <a:fld id="{2C66A066-830F-4C51-9B22-4F499CC843A6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13105,7 +13105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1940F36-644C-421C-A077-691E2C3A9749}" type="CELLRANGE">
+                    <a:fld id="{7985404B-8AA8-4799-90CE-22856E88AB7D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13139,7 +13139,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DB740F6-4CBA-4987-87F4-7E612A3A6220}" type="CELLRANGE">
+                    <a:fld id="{9D6E8A6E-8344-46B3-BDC5-688E9C77D60A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15034,7 +15034,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Noise Function File Type</a:t>
+                  <a:t>Noise Function Language</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -15659,7 +15659,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Noise Function File Type</a:t>
+                  <a:t>Noise Function Language</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -18728,7 +18728,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AC6BF0A-1D79-44D0-A9C3-C80D9FBBA16B}" type="CELLRANGE">
+                    <a:fld id="{C329B3C7-8F14-42AB-AC88-77C75CBC36DF}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18762,7 +18762,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D7AF064-A05B-42A5-900F-BB451F84457F}" type="CELLRANGE">
+                    <a:fld id="{1C0A0F42-5D13-4137-99C3-E354646C1355}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18796,7 +18796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{064B2D41-7FDE-4F76-A073-2E41E82E220E}" type="CELLRANGE">
+                    <a:fld id="{B4095796-0682-437A-A45B-2DE03641BBFC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -35017,8 +35017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668D4FD2-0EC3-4246-9368-74132FA6B2E6}">
   <dimension ref="C3:BH218"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH141" sqref="AH141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69221,7 +69221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E664B0-D829-4FE8-A84D-A0266DB19E99}">
   <dimension ref="A1:AM16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>